<commit_message>
Add filter by tipe dan kriteria ppks
</commit_message>
<xml_diff>
--- a/template/BPJS/format usulan pengaktifan tmt periode januari.xlsx
+++ b/template/BPJS/format usulan pengaktifan tmt periode januari.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\simdata-sosial\template\BPJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523519D7-0036-4DCE-8366-A68CEFE2A9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D47C95-FAE2-4B8B-8D4B-95D06D7F6D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{157B2A51-41F1-4BBB-A2E6-BD4E57291705}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{157B2A51-41F1-4BBB-A2E6-BD4E57291705}"/>
   </bookViews>
   <sheets>
     <sheet name="November" sheetId="2" r:id="rId1"/>
@@ -62,10 +62,16 @@
     <t>STATUS NIKAH</t>
   </si>
   <si>
+    <t>Alamat Tempat Tinggal</t>
+  </si>
+  <si>
     <t>RT</t>
   </si>
   <si>
     <t>RW</t>
+  </si>
+  <si>
+    <t>Kode Pos</t>
   </si>
   <si>
     <t>KECAMATAN</t>
@@ -141,12 +147,6 @@
   </si>
   <si>
     <t>NAMA LENGKAP</t>
-  </si>
-  <si>
-    <t>ALAMAT TEMPAT TINGGAL</t>
-  </si>
-  <si>
-    <t>KODE POS</t>
   </si>
 </sst>
 </file>
@@ -674,7 +674,7 @@
     <xf numFmtId="165" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1300,6 +1300,7 @@
     <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1461,9 +1462,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1501,7 +1502,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1607,7 +1608,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1749,7 +1750,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1759,29 +1760,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856676AE-D3C1-4615-A7E1-28A25E5EF257}">
   <dimension ref="A1:S2169"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="189" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.19921875" customWidth="1"/>
+    <col min="2" max="3" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1328125" customWidth="1"/>
+    <col min="5" max="5" width="13.9296875" customWidth="1"/>
+    <col min="6" max="6" width="15.86328125" style="189" customWidth="1"/>
+    <col min="7" max="7" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.9296875" customWidth="1"/>
+    <col min="9" max="9" width="20.19921875" customWidth="1"/>
+    <col min="10" max="10" width="4.9296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.53125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
     <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="15.42578125" customWidth="1"/>
-    <col min="17" max="17" width="21.85546875" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" customWidth="1"/>
-    <col min="19" max="19" width="21.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.46484375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15.46484375" customWidth="1"/>
+    <col min="17" max="17" width="21.86328125" customWidth="1"/>
+    <col min="18" max="18" width="94.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -1795,7 +1795,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -1810,37 +1810,37 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>20</v>
+      <c r="R1" s="213" t="s">
+        <v>22</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>21</v>
+      <c r="S1" s="213" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -1848,114 +1848,112 @@
         <v>1</v>
       </c>
       <c r="B2" s="190" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="181" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="181" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="181" t="s">
+      <c r="O2" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>29</v>
       </c>
       <c r="P2" s="12">
         <v>2023</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>22</v>
+      <c r="R2" t="s">
+        <v>24</v>
       </c>
-      <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="190" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C3" s="190" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="181" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="181" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>16</v>
-      </c>
       <c r="O3" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P3" s="12">
         <v>2023</v>
       </c>
       <c r="Q3" s="14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>22</v>
+      <c r="R3" t="s">
+        <v>24</v>
       </c>
-      <c r="S3" s="1"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="1"/>
@@ -1975,8 +1973,6 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="14"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="1"/>
@@ -1996,8 +1992,6 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="14"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="1"/>
@@ -2017,8 +2011,6 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="14"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="1"/>
@@ -2038,8 +2030,6 @@
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="14"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="1"/>
@@ -2059,8 +2049,6 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="14"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="1"/>
@@ -2080,8 +2068,6 @@
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="1"/>
@@ -2101,8 +2087,6 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="13"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="1"/>
@@ -2122,8 +2106,6 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="13"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="1"/>
@@ -2143,8 +2125,6 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="13"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="1"/>
@@ -2164,8 +2144,6 @@
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="13"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="1"/>
@@ -2185,8 +2163,6 @@
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="13"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="1"/>
@@ -2206,8 +2182,6 @@
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="1"/>
@@ -2227,10 +2201,8 @@
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="13"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-    </row>
-    <row r="17" spans="1:19">
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="1"/>
       <c r="B17" s="191"/>
       <c r="C17" s="191"/>
@@ -2248,10 +2220,8 @@
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="13"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-    </row>
-    <row r="18" spans="1:19">
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="1"/>
       <c r="B18" s="191"/>
       <c r="C18" s="191"/>
@@ -2269,10 +2239,8 @@
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="13"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-    </row>
-    <row r="19" spans="1:19">
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="1"/>
       <c r="B19" s="191"/>
       <c r="C19" s="191"/>
@@ -2290,10 +2258,8 @@
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="13"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-    </row>
-    <row r="20" spans="1:19">
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="1"/>
       <c r="B20" s="191"/>
       <c r="C20" s="191"/>
@@ -2311,10 +2277,8 @@
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="13"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-    </row>
-    <row r="21" spans="1:19">
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="1"/>
       <c r="B21" s="191"/>
       <c r="C21" s="191"/>
@@ -2332,10 +2296,8 @@
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="13"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-    </row>
-    <row r="22" spans="1:19">
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" s="1"/>
       <c r="B22" s="191"/>
       <c r="C22" s="191"/>
@@ -2353,10 +2315,8 @@
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="13"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19">
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="1"/>
       <c r="B23" s="191"/>
       <c r="C23" s="191"/>
@@ -2374,10 +2334,8 @@
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="13"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-    </row>
-    <row r="24" spans="1:19">
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="1"/>
       <c r="B24" s="191"/>
       <c r="C24" s="191"/>
@@ -2395,10 +2353,8 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="13"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-    </row>
-    <row r="25" spans="1:19">
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" s="1"/>
       <c r="B25" s="191"/>
       <c r="C25" s="191"/>
@@ -2416,10 +2372,8 @@
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="13"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-    </row>
-    <row r="26" spans="1:19">
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" s="1"/>
       <c r="B26" s="191"/>
       <c r="C26" s="191"/>
@@ -2437,10 +2391,8 @@
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="13"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-    </row>
-    <row r="27" spans="1:19">
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" s="1"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -2458,10 +2410,8 @@
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="14"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-    </row>
-    <row r="28" spans="1:19">
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" s="1"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -2479,10 +2429,8 @@
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
       <c r="Q28" s="14"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-    </row>
-    <row r="29" spans="1:19">
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="1"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -2500,10 +2448,8 @@
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="14"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-    </row>
-    <row r="30" spans="1:19">
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" s="1"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -2521,16 +2467,14 @@
       <c r="O30" s="12"/>
       <c r="P30" s="12"/>
       <c r="Q30" s="14"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-    </row>
-    <row r="31" spans="1:19">
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" s="1"/>
       <c r="B31" s="192"/>
       <c r="C31" s="3"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="213"/>
+      <c r="F31" s="214"/>
       <c r="G31" s="35"/>
       <c r="H31" s="35"/>
       <c r="I31" s="14"/>
@@ -2542,16 +2486,14 @@
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
       <c r="Q31" s="14"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-    </row>
-    <row r="32" spans="1:19">
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32" s="1"/>
       <c r="B32" s="192"/>
       <c r="C32" s="3"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
-      <c r="F32" s="213"/>
+      <c r="F32" s="214"/>
       <c r="G32" s="35"/>
       <c r="H32" s="35"/>
       <c r="I32" s="14"/>
@@ -2563,16 +2505,14 @@
       <c r="O32" s="12"/>
       <c r="P32" s="12"/>
       <c r="Q32" s="14"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-    </row>
-    <row r="33" spans="1:19">
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33" s="1"/>
       <c r="B33" s="192"/>
       <c r="C33" s="3"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
-      <c r="F33" s="213"/>
+      <c r="F33" s="214"/>
       <c r="G33" s="35"/>
       <c r="H33" s="35"/>
       <c r="I33" s="14"/>
@@ -2584,16 +2524,14 @@
       <c r="O33" s="12"/>
       <c r="P33" s="12"/>
       <c r="Q33" s="14"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-    </row>
-    <row r="34" spans="1:19">
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34" s="1"/>
       <c r="B34" s="3"/>
       <c r="C34" s="192"/>
       <c r="D34" s="13"/>
       <c r="E34" s="6"/>
-      <c r="F34" s="213"/>
+      <c r="F34" s="214"/>
       <c r="G34" s="35"/>
       <c r="H34" s="35"/>
       <c r="I34" s="14"/>
@@ -2605,16 +2543,14 @@
       <c r="O34" s="12"/>
       <c r="P34" s="12"/>
       <c r="Q34" s="14"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-    </row>
-    <row r="35" spans="1:19">
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35" s="1"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
-      <c r="F35" s="213"/>
+      <c r="F35" s="214"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
       <c r="I35" s="14"/>
@@ -2626,16 +2562,14 @@
       <c r="O35" s="12"/>
       <c r="P35" s="12"/>
       <c r="Q35" s="14"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-    </row>
-    <row r="36" spans="1:19">
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36" s="1"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
-      <c r="F36" s="213"/>
+      <c r="F36" s="214"/>
       <c r="G36" s="35"/>
       <c r="H36" s="35"/>
       <c r="I36" s="14"/>
@@ -2647,16 +2581,14 @@
       <c r="O36" s="12"/>
       <c r="P36" s="12"/>
       <c r="Q36" s="14"/>
-      <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-    </row>
-    <row r="37" spans="1:19">
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37" s="1"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="213"/>
+      <c r="F37" s="214"/>
       <c r="G37" s="35"/>
       <c r="H37" s="35"/>
       <c r="I37" s="14"/>
@@ -2668,16 +2600,14 @@
       <c r="O37" s="12"/>
       <c r="P37" s="12"/>
       <c r="Q37" s="14"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-    </row>
-    <row r="38" spans="1:19">
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38" s="1"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="213"/>
+      <c r="F38" s="214"/>
       <c r="G38" s="35"/>
       <c r="H38" s="35"/>
       <c r="I38" s="14"/>
@@ -2689,16 +2619,14 @@
       <c r="O38" s="12"/>
       <c r="P38" s="12"/>
       <c r="Q38" s="14"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-    </row>
-    <row r="39" spans="1:19">
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" s="1"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
-      <c r="F39" s="213"/>
+      <c r="F39" s="214"/>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
       <c r="I39" s="14"/>
@@ -2710,10 +2638,8 @@
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
       <c r="Q39" s="14"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-    </row>
-    <row r="40" spans="1:19">
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40" s="1"/>
       <c r="B40" s="192"/>
       <c r="C40" s="3"/>
@@ -2731,10 +2657,8 @@
       <c r="O40" s="12"/>
       <c r="P40" s="12"/>
       <c r="Q40" s="14"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-    </row>
-    <row r="41" spans="1:19">
+    </row>
+    <row r="41" spans="1:17">
       <c r="A41" s="1"/>
       <c r="B41" s="192"/>
       <c r="C41" s="191"/>
@@ -2752,10 +2676,8 @@
       <c r="O41" s="12"/>
       <c r="P41" s="12"/>
       <c r="Q41" s="13"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-    </row>
-    <row r="42" spans="1:19">
+    </row>
+    <row r="42" spans="1:17">
       <c r="A42" s="1"/>
       <c r="B42" s="192"/>
       <c r="C42" s="191"/>
@@ -2773,10 +2695,8 @@
       <c r="O42" s="12"/>
       <c r="P42" s="12"/>
       <c r="Q42" s="13"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-    </row>
-    <row r="43" spans="1:19">
+    </row>
+    <row r="43" spans="1:17">
       <c r="A43" s="1"/>
       <c r="B43" s="192"/>
       <c r="C43" s="191"/>
@@ -2794,10 +2714,8 @@
       <c r="O43" s="12"/>
       <c r="P43" s="12"/>
       <c r="Q43" s="13"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-    </row>
-    <row r="44" spans="1:19">
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44" s="1"/>
       <c r="B44" s="192"/>
       <c r="C44" s="3"/>
@@ -2815,10 +2733,8 @@
       <c r="O44" s="12"/>
       <c r="P44" s="12"/>
       <c r="Q44" s="14"/>
-      <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
-    </row>
-    <row r="45" spans="1:19">
+    </row>
+    <row r="45" spans="1:17">
       <c r="A45" s="1"/>
       <c r="B45" s="191"/>
       <c r="C45" s="191"/>
@@ -2836,10 +2752,8 @@
       <c r="O45" s="12"/>
       <c r="P45" s="12"/>
       <c r="Q45" s="13"/>
-      <c r="R45" s="1"/>
-      <c r="S45" s="1"/>
-    </row>
-    <row r="46" spans="1:19">
+    </row>
+    <row r="46" spans="1:17">
       <c r="A46" s="1"/>
       <c r="B46" s="191"/>
       <c r="C46" s="191"/>
@@ -2857,10 +2771,8 @@
       <c r="O46" s="12"/>
       <c r="P46" s="12"/>
       <c r="Q46" s="13"/>
-      <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-    </row>
-    <row r="47" spans="1:19">
+    </row>
+    <row r="47" spans="1:17">
       <c r="A47" s="1"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2878,10 +2790,8 @@
       <c r="O47" s="12"/>
       <c r="P47" s="12"/>
       <c r="Q47" s="13"/>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-    </row>
-    <row r="48" spans="1:19">
+    </row>
+    <row r="48" spans="1:17">
       <c r="A48" s="1"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2899,10 +2809,8 @@
       <c r="O48" s="12"/>
       <c r="P48" s="12"/>
       <c r="Q48" s="13"/>
-      <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
-    </row>
-    <row r="49" spans="1:19">
+    </row>
+    <row r="49" spans="1:17">
       <c r="A49" s="1"/>
       <c r="B49" s="191"/>
       <c r="C49" s="191"/>
@@ -2920,10 +2828,8 @@
       <c r="O49" s="12"/>
       <c r="P49" s="12"/>
       <c r="Q49" s="13"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-    </row>
-    <row r="50" spans="1:19">
+    </row>
+    <row r="50" spans="1:17">
       <c r="A50" s="1"/>
       <c r="B50" s="191"/>
       <c r="C50" s="191"/>
@@ -2941,10 +2847,8 @@
       <c r="O50" s="12"/>
       <c r="P50" s="12"/>
       <c r="Q50" s="13"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
-    </row>
-    <row r="51" spans="1:19">
+    </row>
+    <row r="51" spans="1:17">
       <c r="A51" s="1"/>
       <c r="B51" s="191"/>
       <c r="C51" s="191"/>
@@ -2962,10 +2866,8 @@
       <c r="O51" s="12"/>
       <c r="P51" s="12"/>
       <c r="Q51" s="13"/>
-      <c r="R51" s="1"/>
-      <c r="S51" s="1"/>
-    </row>
-    <row r="52" spans="1:19">
+    </row>
+    <row r="52" spans="1:17">
       <c r="A52" s="1"/>
       <c r="B52" s="191"/>
       <c r="C52" s="191"/>
@@ -2983,10 +2885,8 @@
       <c r="O52" s="12"/>
       <c r="P52" s="12"/>
       <c r="Q52" s="13"/>
-      <c r="R52" s="1"/>
-      <c r="S52" s="1"/>
-    </row>
-    <row r="53" spans="1:19">
+    </row>
+    <row r="53" spans="1:17">
       <c r="A53" s="1"/>
       <c r="B53" s="191"/>
       <c r="C53" s="191"/>
@@ -3004,10 +2904,8 @@
       <c r="O53" s="12"/>
       <c r="P53" s="12"/>
       <c r="Q53" s="13"/>
-      <c r="R53" s="1"/>
-      <c r="S53" s="1"/>
-    </row>
-    <row r="54" spans="1:19">
+    </row>
+    <row r="54" spans="1:17">
       <c r="A54" s="1"/>
       <c r="B54" s="191"/>
       <c r="C54" s="191"/>
@@ -3025,10 +2923,8 @@
       <c r="O54" s="12"/>
       <c r="P54" s="12"/>
       <c r="Q54" s="13"/>
-      <c r="R54" s="1"/>
-      <c r="S54" s="1"/>
-    </row>
-    <row r="55" spans="1:19">
+    </row>
+    <row r="55" spans="1:17">
       <c r="A55" s="1"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -3046,10 +2942,8 @@
       <c r="O55" s="12"/>
       <c r="P55" s="12"/>
       <c r="Q55" s="14"/>
-      <c r="R55" s="1"/>
-      <c r="S55" s="1"/>
-    </row>
-    <row r="56" spans="1:19">
+    </row>
+    <row r="56" spans="1:17">
       <c r="A56" s="1"/>
       <c r="B56" s="191"/>
       <c r="C56" s="191"/>
@@ -3067,10 +2961,8 @@
       <c r="O56" s="12"/>
       <c r="P56" s="12"/>
       <c r="Q56" s="13"/>
-      <c r="R56" s="1"/>
-      <c r="S56" s="1"/>
-    </row>
-    <row r="57" spans="1:19">
+    </row>
+    <row r="57" spans="1:17">
       <c r="A57" s="1"/>
       <c r="B57" s="191"/>
       <c r="C57" s="191"/>
@@ -3088,10 +2980,8 @@
       <c r="O57" s="12"/>
       <c r="P57" s="12"/>
       <c r="Q57" s="13"/>
-      <c r="R57" s="1"/>
-      <c r="S57" s="1"/>
-    </row>
-    <row r="58" spans="1:19">
+    </row>
+    <row r="58" spans="1:17">
       <c r="A58" s="1"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -3109,10 +2999,8 @@
       <c r="O58" s="12"/>
       <c r="P58" s="12"/>
       <c r="Q58" s="14"/>
-      <c r="R58" s="1"/>
-      <c r="S58" s="1"/>
-    </row>
-    <row r="59" spans="1:19">
+    </row>
+    <row r="59" spans="1:17">
       <c r="A59" s="1"/>
       <c r="B59" s="191"/>
       <c r="C59" s="191"/>
@@ -3130,10 +3018,8 @@
       <c r="O59" s="12"/>
       <c r="P59" s="12"/>
       <c r="Q59" s="14"/>
-      <c r="R59" s="1"/>
-      <c r="S59" s="1"/>
-    </row>
-    <row r="60" spans="1:19">
+    </row>
+    <row r="60" spans="1:17">
       <c r="A60" s="1"/>
       <c r="B60" s="191"/>
       <c r="C60" s="191"/>
@@ -3151,10 +3037,8 @@
       <c r="O60" s="12"/>
       <c r="P60" s="12"/>
       <c r="Q60" s="14"/>
-      <c r="R60" s="1"/>
-      <c r="S60" s="1"/>
-    </row>
-    <row r="61" spans="1:19">
+    </row>
+    <row r="61" spans="1:17">
       <c r="A61" s="1"/>
       <c r="B61" s="191"/>
       <c r="C61" s="191"/>
@@ -3172,10 +3056,8 @@
       <c r="O61" s="12"/>
       <c r="P61" s="12"/>
       <c r="Q61" s="14"/>
-      <c r="R61" s="1"/>
-      <c r="S61" s="1"/>
-    </row>
-    <row r="62" spans="1:19">
+    </row>
+    <row r="62" spans="1:17">
       <c r="A62" s="1"/>
       <c r="B62" s="191"/>
       <c r="C62" s="191"/>
@@ -3193,16 +3075,14 @@
       <c r="O62" s="12"/>
       <c r="P62" s="12"/>
       <c r="Q62" s="14"/>
-      <c r="R62" s="1"/>
-      <c r="S62" s="1"/>
-    </row>
-    <row r="63" spans="1:19">
+    </row>
+    <row r="63" spans="1:17">
       <c r="A63" s="1"/>
       <c r="B63" s="193"/>
       <c r="C63" s="193"/>
       <c r="D63" s="15"/>
       <c r="E63" s="15"/>
-      <c r="F63" s="214"/>
+      <c r="F63" s="215"/>
       <c r="G63" s="35"/>
       <c r="H63" s="37"/>
       <c r="I63" s="15"/>
@@ -3214,16 +3094,14 @@
       <c r="O63" s="12"/>
       <c r="P63" s="12"/>
       <c r="Q63" s="3"/>
-      <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
-    </row>
-    <row r="64" spans="1:19">
+    </row>
+    <row r="64" spans="1:17">
       <c r="A64" s="1"/>
       <c r="B64" s="193"/>
       <c r="C64" s="193"/>
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
-      <c r="F64" s="214"/>
+      <c r="F64" s="215"/>
       <c r="G64" s="35"/>
       <c r="H64" s="37"/>
       <c r="I64" s="15"/>
@@ -3235,16 +3113,14 @@
       <c r="O64" s="12"/>
       <c r="P64" s="12"/>
       <c r="Q64" s="3"/>
-      <c r="R64" s="1"/>
-      <c r="S64" s="1"/>
-    </row>
-    <row r="65" spans="1:19">
+    </row>
+    <row r="65" spans="1:17">
       <c r="A65" s="1"/>
       <c r="B65" s="193"/>
       <c r="C65" s="193"/>
       <c r="D65" s="15"/>
       <c r="E65" s="15"/>
-      <c r="F65" s="214"/>
+      <c r="F65" s="215"/>
       <c r="G65" s="35"/>
       <c r="H65" s="38"/>
       <c r="I65" s="15"/>
@@ -3256,10 +3132,8 @@
       <c r="O65" s="12"/>
       <c r="P65" s="12"/>
       <c r="Q65" s="3"/>
-      <c r="R65" s="1"/>
-      <c r="S65" s="1"/>
-    </row>
-    <row r="66" spans="1:19">
+    </row>
+    <row r="66" spans="1:17">
       <c r="A66" s="1"/>
       <c r="B66" s="193"/>
       <c r="C66" s="191"/>
@@ -3277,16 +3151,14 @@
       <c r="O66" s="12"/>
       <c r="P66" s="12"/>
       <c r="Q66" s="3"/>
-      <c r="R66" s="1"/>
-      <c r="S66" s="1"/>
-    </row>
-    <row r="67" spans="1:19">
+    </row>
+    <row r="67" spans="1:17">
       <c r="A67" s="1"/>
       <c r="B67" s="194"/>
       <c r="C67" s="194"/>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
-      <c r="F67" s="215"/>
+      <c r="F67" s="216"/>
       <c r="G67" s="35"/>
       <c r="H67" s="36"/>
       <c r="I67" s="16"/>
@@ -3298,16 +3170,14 @@
       <c r="O67" s="12"/>
       <c r="P67" s="12"/>
       <c r="Q67" s="13"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
-    </row>
-    <row r="68" spans="1:19">
+    </row>
+    <row r="68" spans="1:17">
       <c r="A68" s="1"/>
       <c r="B68" s="194"/>
       <c r="C68" s="194"/>
       <c r="D68" s="16"/>
       <c r="E68" s="16"/>
-      <c r="F68" s="215"/>
+      <c r="F68" s="216"/>
       <c r="G68" s="35"/>
       <c r="H68" s="36"/>
       <c r="I68" s="16"/>
@@ -3319,16 +3189,14 @@
       <c r="O68" s="12"/>
       <c r="P68" s="12"/>
       <c r="Q68" s="13"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
-    </row>
-    <row r="69" spans="1:19">
+    </row>
+    <row r="69" spans="1:17">
       <c r="A69" s="1"/>
       <c r="B69" s="194"/>
       <c r="C69" s="194"/>
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
-      <c r="F69" s="215"/>
+      <c r="F69" s="216"/>
       <c r="G69" s="35"/>
       <c r="H69" s="36"/>
       <c r="I69" s="16"/>
@@ -3340,10 +3208,8 @@
       <c r="O69" s="12"/>
       <c r="P69" s="12"/>
       <c r="Q69" s="13"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-    </row>
-    <row r="70" spans="1:19">
+    </row>
+    <row r="70" spans="1:17">
       <c r="A70" s="1"/>
       <c r="B70" s="184"/>
       <c r="C70" s="184"/>
@@ -3361,10 +3227,8 @@
       <c r="O70" s="12"/>
       <c r="P70" s="12"/>
       <c r="Q70" s="23"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
-    </row>
-    <row r="71" spans="1:19">
+    </row>
+    <row r="71" spans="1:17">
       <c r="A71" s="1"/>
       <c r="B71" s="184"/>
       <c r="C71" s="184"/>
@@ -3382,10 +3246,8 @@
       <c r="O71" s="12"/>
       <c r="P71" s="12"/>
       <c r="Q71" s="23"/>
-      <c r="R71" s="1"/>
-      <c r="S71" s="1"/>
-    </row>
-    <row r="72" spans="1:19">
+    </row>
+    <row r="72" spans="1:17">
       <c r="A72" s="1"/>
       <c r="B72" s="184"/>
       <c r="C72" s="184"/>
@@ -3403,10 +3265,8 @@
       <c r="O72" s="12"/>
       <c r="P72" s="12"/>
       <c r="Q72" s="23"/>
-      <c r="R72" s="1"/>
-      <c r="S72" s="1"/>
-    </row>
-    <row r="73" spans="1:19">
+    </row>
+    <row r="73" spans="1:17">
       <c r="A73" s="1"/>
       <c r="B73" s="184"/>
       <c r="C73" s="184"/>
@@ -3424,10 +3284,8 @@
       <c r="O73" s="12"/>
       <c r="P73" s="12"/>
       <c r="Q73" s="23"/>
-      <c r="R73" s="1"/>
-      <c r="S73" s="1"/>
-    </row>
-    <row r="74" spans="1:19">
+    </row>
+    <row r="74" spans="1:17">
       <c r="A74" s="1"/>
       <c r="B74" s="184"/>
       <c r="C74" s="184"/>
@@ -3445,10 +3303,8 @@
       <c r="O74" s="12"/>
       <c r="P74" s="12"/>
       <c r="Q74" s="23"/>
-      <c r="R74" s="1"/>
-      <c r="S74" s="1"/>
-    </row>
-    <row r="75" spans="1:19">
+    </row>
+    <row r="75" spans="1:17">
       <c r="A75" s="1"/>
       <c r="B75" s="184"/>
       <c r="C75" s="184"/>
@@ -3466,10 +3322,8 @@
       <c r="O75" s="12"/>
       <c r="P75" s="12"/>
       <c r="Q75" s="23"/>
-      <c r="R75" s="1"/>
-      <c r="S75" s="1"/>
-    </row>
-    <row r="76" spans="1:19">
+    </row>
+    <row r="76" spans="1:17">
       <c r="A76" s="1"/>
       <c r="B76" s="184"/>
       <c r="C76" s="184"/>
@@ -3487,10 +3341,8 @@
       <c r="O76" s="12"/>
       <c r="P76" s="12"/>
       <c r="Q76" s="23"/>
-      <c r="R76" s="1"/>
-      <c r="S76" s="1"/>
-    </row>
-    <row r="77" spans="1:19">
+    </row>
+    <row r="77" spans="1:17">
       <c r="A77" s="1"/>
       <c r="B77" s="184"/>
       <c r="C77" s="184"/>
@@ -3508,10 +3360,8 @@
       <c r="O77" s="12"/>
       <c r="P77" s="12"/>
       <c r="Q77" s="23"/>
-      <c r="R77" s="1"/>
-      <c r="S77" s="1"/>
-    </row>
-    <row r="78" spans="1:19">
+    </row>
+    <row r="78" spans="1:17">
       <c r="A78" s="1"/>
       <c r="B78" s="184"/>
       <c r="C78" s="184"/>
@@ -3529,10 +3379,8 @@
       <c r="O78" s="12"/>
       <c r="P78" s="12"/>
       <c r="Q78" s="23"/>
-      <c r="R78" s="1"/>
-      <c r="S78" s="1"/>
-    </row>
-    <row r="79" spans="1:19">
+    </row>
+    <row r="79" spans="1:17">
       <c r="A79" s="1"/>
       <c r="B79" s="184"/>
       <c r="C79" s="184"/>
@@ -3550,10 +3398,8 @@
       <c r="O79" s="12"/>
       <c r="P79" s="12"/>
       <c r="Q79" s="23"/>
-      <c r="R79" s="1"/>
-      <c r="S79" s="1"/>
-    </row>
-    <row r="80" spans="1:19">
+    </row>
+    <row r="80" spans="1:17">
       <c r="A80" s="1"/>
       <c r="B80" s="184"/>
       <c r="C80" s="184"/>
@@ -3571,10 +3417,8 @@
       <c r="O80" s="12"/>
       <c r="P80" s="12"/>
       <c r="Q80" s="23"/>
-      <c r="R80" s="1"/>
-      <c r="S80" s="1"/>
-    </row>
-    <row r="81" spans="1:19">
+    </row>
+    <row r="81" spans="1:17">
       <c r="A81" s="1"/>
       <c r="B81" s="184"/>
       <c r="C81" s="184"/>
@@ -3592,10 +3436,8 @@
       <c r="O81" s="12"/>
       <c r="P81" s="12"/>
       <c r="Q81" s="23"/>
-      <c r="R81" s="1"/>
-      <c r="S81" s="1"/>
-    </row>
-    <row r="82" spans="1:19">
+    </row>
+    <row r="82" spans="1:17">
       <c r="A82" s="1"/>
       <c r="B82" s="184"/>
       <c r="C82" s="184"/>
@@ -3613,10 +3455,8 @@
       <c r="O82" s="12"/>
       <c r="P82" s="12"/>
       <c r="Q82" s="23"/>
-      <c r="R82" s="1"/>
-      <c r="S82" s="1"/>
-    </row>
-    <row r="83" spans="1:19">
+    </row>
+    <row r="83" spans="1:17">
       <c r="A83" s="1"/>
       <c r="B83" s="184"/>
       <c r="C83" s="184"/>
@@ -3634,10 +3474,8 @@
       <c r="O83" s="12"/>
       <c r="P83" s="12"/>
       <c r="Q83" s="23"/>
-      <c r="R83" s="1"/>
-      <c r="S83" s="1"/>
-    </row>
-    <row r="84" spans="1:19">
+    </row>
+    <row r="84" spans="1:17">
       <c r="A84" s="1"/>
       <c r="B84" s="184"/>
       <c r="C84" s="184"/>
@@ -3655,10 +3493,8 @@
       <c r="O84" s="12"/>
       <c r="P84" s="12"/>
       <c r="Q84" s="23"/>
-      <c r="R84" s="1"/>
-      <c r="S84" s="1"/>
-    </row>
-    <row r="85" spans="1:19">
+    </row>
+    <row r="85" spans="1:17">
       <c r="A85" s="1"/>
       <c r="B85" s="184"/>
       <c r="C85" s="184"/>
@@ -3676,10 +3512,8 @@
       <c r="O85" s="12"/>
       <c r="P85" s="12"/>
       <c r="Q85" s="23"/>
-      <c r="R85" s="1"/>
-      <c r="S85" s="1"/>
-    </row>
-    <row r="86" spans="1:19">
+    </row>
+    <row r="86" spans="1:17">
       <c r="A86" s="1"/>
       <c r="B86" s="184"/>
       <c r="C86" s="184"/>
@@ -3697,10 +3531,8 @@
       <c r="O86" s="12"/>
       <c r="P86" s="12"/>
       <c r="Q86" s="23"/>
-      <c r="R86" s="1"/>
-      <c r="S86" s="1"/>
-    </row>
-    <row r="87" spans="1:19">
+    </row>
+    <row r="87" spans="1:17">
       <c r="A87" s="1"/>
       <c r="B87" s="184"/>
       <c r="C87" s="184"/>
@@ -3718,10 +3550,8 @@
       <c r="O87" s="12"/>
       <c r="P87" s="12"/>
       <c r="Q87" s="23"/>
-      <c r="R87" s="1"/>
-      <c r="S87" s="1"/>
-    </row>
-    <row r="88" spans="1:19">
+    </row>
+    <row r="88" spans="1:17">
       <c r="A88" s="1"/>
       <c r="B88" s="184"/>
       <c r="C88" s="184"/>
@@ -3739,10 +3569,8 @@
       <c r="O88" s="12"/>
       <c r="P88" s="12"/>
       <c r="Q88" s="23"/>
-      <c r="R88" s="1"/>
-      <c r="S88" s="1"/>
-    </row>
-    <row r="89" spans="1:19">
+    </row>
+    <row r="89" spans="1:17">
       <c r="A89" s="1"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -3760,10 +3588,8 @@
       <c r="O89" s="12"/>
       <c r="P89" s="12"/>
       <c r="Q89" s="5"/>
-      <c r="R89" s="1"/>
-      <c r="S89" s="1"/>
-    </row>
-    <row r="90" spans="1:19">
+    </row>
+    <row r="90" spans="1:17">
       <c r="A90" s="1"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
@@ -3781,10 +3607,8 @@
       <c r="O90" s="12"/>
       <c r="P90" s="12"/>
       <c r="Q90" s="5"/>
-      <c r="R90" s="1"/>
-      <c r="S90" s="1"/>
-    </row>
-    <row r="91" spans="1:19">
+    </row>
+    <row r="91" spans="1:17">
       <c r="A91" s="1"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
@@ -3803,7 +3627,7 @@
       <c r="P91" s="12"/>
       <c r="Q91" s="5"/>
     </row>
-    <row r="92" spans="1:19">
+    <row r="92" spans="1:17">
       <c r="A92" s="1"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
@@ -3822,13 +3646,13 @@
       <c r="P92" s="12"/>
       <c r="Q92" s="5"/>
     </row>
-    <row r="93" spans="1:19">
+    <row r="93" spans="1:17">
       <c r="A93" s="1"/>
       <c r="B93" s="195"/>
       <c r="C93" s="195"/>
       <c r="D93" s="17"/>
       <c r="E93" s="18"/>
-      <c r="F93" s="216"/>
+      <c r="F93" s="217"/>
       <c r="G93" s="35"/>
       <c r="H93" s="37"/>
       <c r="I93" s="45"/>
@@ -3841,13 +3665,13 @@
       <c r="P93" s="12"/>
       <c r="Q93" s="14"/>
     </row>
-    <row r="94" spans="1:19">
+    <row r="94" spans="1:17">
       <c r="A94" s="1"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="14"/>
       <c r="E94" s="6"/>
-      <c r="F94" s="213"/>
+      <c r="F94" s="214"/>
       <c r="G94" s="35"/>
       <c r="H94" s="37"/>
       <c r="I94" s="19"/>
@@ -3860,13 +3684,13 @@
       <c r="P94" s="12"/>
       <c r="Q94" s="14"/>
     </row>
-    <row r="95" spans="1:19">
+    <row r="95" spans="1:17">
       <c r="A95" s="1"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="18"/>
       <c r="E95" s="6"/>
-      <c r="F95" s="213"/>
+      <c r="F95" s="214"/>
       <c r="G95" s="35"/>
       <c r="H95" s="37"/>
       <c r="I95" s="19"/>
@@ -3879,13 +3703,13 @@
       <c r="P95" s="12"/>
       <c r="Q95" s="14"/>
     </row>
-    <row r="96" spans="1:19">
+    <row r="96" spans="1:17">
       <c r="A96" s="1"/>
       <c r="B96" s="196"/>
       <c r="C96" s="196"/>
       <c r="D96" s="17"/>
       <c r="E96" s="18"/>
-      <c r="F96" s="216"/>
+      <c r="F96" s="217"/>
       <c r="G96" s="35"/>
       <c r="H96" s="37"/>
       <c r="I96" s="46"/>
@@ -3923,7 +3747,7 @@
       <c r="C98" s="208"/>
       <c r="D98" s="185"/>
       <c r="E98" s="29"/>
-      <c r="F98" s="217"/>
+      <c r="F98" s="218"/>
       <c r="G98" s="35"/>
       <c r="H98" s="40"/>
       <c r="I98" s="29"/>
@@ -5937,7 +5761,7 @@
       <c r="C204" s="6"/>
       <c r="D204" s="6"/>
       <c r="E204" s="6"/>
-      <c r="F204" s="213"/>
+      <c r="F204" s="214"/>
       <c r="G204" s="35"/>
       <c r="H204" s="44"/>
       <c r="I204" s="6"/>
@@ -5956,7 +5780,7 @@
       <c r="C205" s="6"/>
       <c r="D205" s="6"/>
       <c r="E205" s="6"/>
-      <c r="F205" s="213"/>
+      <c r="F205" s="214"/>
       <c r="G205" s="35"/>
       <c r="H205" s="44"/>
       <c r="I205" s="6"/>
@@ -5975,7 +5799,7 @@
       <c r="C206" s="6"/>
       <c r="D206" s="6"/>
       <c r="E206" s="6"/>
-      <c r="F206" s="213"/>
+      <c r="F206" s="214"/>
       <c r="G206" s="35"/>
       <c r="H206" s="44"/>
       <c r="I206" s="6"/>
@@ -5994,7 +5818,7 @@
       <c r="C207" s="6"/>
       <c r="D207" s="6"/>
       <c r="E207" s="6"/>
-      <c r="F207" s="213"/>
+      <c r="F207" s="214"/>
       <c r="G207" s="35"/>
       <c r="H207" s="44"/>
       <c r="I207" s="6"/>
@@ -6013,7 +5837,7 @@
       <c r="C208" s="6"/>
       <c r="D208" s="6"/>
       <c r="E208" s="6"/>
-      <c r="F208" s="213"/>
+      <c r="F208" s="214"/>
       <c r="G208" s="35"/>
       <c r="H208" s="35"/>
       <c r="I208" s="6"/>
@@ -6032,7 +5856,7 @@
       <c r="C209" s="6"/>
       <c r="D209" s="6"/>
       <c r="E209" s="6"/>
-      <c r="F209" s="213"/>
+      <c r="F209" s="214"/>
       <c r="G209" s="35"/>
       <c r="H209" s="44"/>
       <c r="I209" s="6"/>
@@ -6051,7 +5875,7 @@
       <c r="C210" s="6"/>
       <c r="D210" s="6"/>
       <c r="E210" s="6"/>
-      <c r="F210" s="213"/>
+      <c r="F210" s="214"/>
       <c r="G210" s="35"/>
       <c r="H210" s="44"/>
       <c r="I210" s="6"/>
@@ -6070,7 +5894,7 @@
       <c r="C211" s="6"/>
       <c r="D211" s="6"/>
       <c r="E211" s="6"/>
-      <c r="F211" s="213"/>
+      <c r="F211" s="214"/>
       <c r="G211" s="35"/>
       <c r="H211" s="44"/>
       <c r="I211" s="6"/>
@@ -6089,7 +5913,7 @@
       <c r="C212" s="6"/>
       <c r="D212" s="6"/>
       <c r="E212" s="6"/>
-      <c r="F212" s="213"/>
+      <c r="F212" s="214"/>
       <c r="G212" s="35"/>
       <c r="H212" s="44"/>
       <c r="I212" s="6"/>
@@ -6108,7 +5932,7 @@
       <c r="C213" s="6"/>
       <c r="D213" s="6"/>
       <c r="E213" s="6"/>
-      <c r="F213" s="213"/>
+      <c r="F213" s="214"/>
       <c r="G213" s="35"/>
       <c r="H213" s="44"/>
       <c r="I213" s="6"/>
@@ -6127,7 +5951,7 @@
       <c r="C214" s="6"/>
       <c r="D214" s="6"/>
       <c r="E214" s="6"/>
-      <c r="F214" s="213"/>
+      <c r="F214" s="214"/>
       <c r="G214" s="35"/>
       <c r="H214" s="44"/>
       <c r="I214" s="6"/>
@@ -6146,7 +5970,7 @@
       <c r="C215" s="6"/>
       <c r="D215" s="6"/>
       <c r="E215" s="6"/>
-      <c r="F215" s="213"/>
+      <c r="F215" s="214"/>
       <c r="G215" s="35"/>
       <c r="H215" s="44"/>
       <c r="I215" s="6"/>
@@ -6165,7 +5989,7 @@
       <c r="C216" s="202"/>
       <c r="D216" s="18"/>
       <c r="E216" s="18"/>
-      <c r="F216" s="216"/>
+      <c r="F216" s="217"/>
       <c r="G216" s="35"/>
       <c r="H216" s="35"/>
       <c r="I216" s="14"/>
@@ -6393,7 +6217,7 @@
       <c r="C228" s="6"/>
       <c r="D228" s="6"/>
       <c r="E228" s="6"/>
-      <c r="F228" s="213"/>
+      <c r="F228" s="214"/>
       <c r="G228" s="35"/>
       <c r="H228" s="44"/>
       <c r="I228" s="14"/>
@@ -6412,7 +6236,7 @@
       <c r="C229" s="6"/>
       <c r="D229" s="6"/>
       <c r="E229" s="6"/>
-      <c r="F229" s="213"/>
+      <c r="F229" s="214"/>
       <c r="G229" s="35"/>
       <c r="H229" s="44"/>
       <c r="I229" s="14"/>
@@ -6431,7 +6255,7 @@
       <c r="C230" s="202"/>
       <c r="D230" s="18"/>
       <c r="E230" s="18"/>
-      <c r="F230" s="216"/>
+      <c r="F230" s="217"/>
       <c r="G230" s="35"/>
       <c r="H230" s="35"/>
       <c r="I230" s="14"/>
@@ -6450,7 +6274,7 @@
       <c r="C231" s="6"/>
       <c r="D231" s="6"/>
       <c r="E231" s="6"/>
-      <c r="F231" s="213"/>
+      <c r="F231" s="214"/>
       <c r="G231" s="35"/>
       <c r="H231" s="44"/>
       <c r="I231" s="6"/>
@@ -6469,7 +6293,7 @@
       <c r="C232" s="6"/>
       <c r="D232" s="6"/>
       <c r="E232" s="6"/>
-      <c r="F232" s="213"/>
+      <c r="F232" s="214"/>
       <c r="G232" s="35"/>
       <c r="H232" s="44"/>
       <c r="I232" s="6"/>
@@ -6488,7 +6312,7 @@
       <c r="C233" s="6"/>
       <c r="D233" s="6"/>
       <c r="E233" s="6"/>
-      <c r="F233" s="213"/>
+      <c r="F233" s="214"/>
       <c r="G233" s="35"/>
       <c r="H233" s="44"/>
       <c r="I233" s="6"/>
@@ -9604,7 +9428,7 @@
       <c r="C397" s="7"/>
       <c r="D397" s="14"/>
       <c r="E397" s="18"/>
-      <c r="F397" s="216"/>
+      <c r="F397" s="217"/>
       <c r="G397" s="35"/>
       <c r="H397" s="37"/>
       <c r="I397" s="19"/>
@@ -10041,7 +9865,7 @@
       <c r="C420" s="3"/>
       <c r="D420" s="18"/>
       <c r="E420" s="18"/>
-      <c r="F420" s="216"/>
+      <c r="F420" s="217"/>
       <c r="G420" s="35"/>
       <c r="H420" s="35"/>
       <c r="I420" s="14"/>
@@ -10060,7 +9884,7 @@
       <c r="C421" s="3"/>
       <c r="D421" s="18"/>
       <c r="E421" s="18"/>
-      <c r="F421" s="216"/>
+      <c r="F421" s="217"/>
       <c r="G421" s="35"/>
       <c r="H421" s="35"/>
       <c r="I421" s="14"/>
@@ -10079,7 +9903,7 @@
       <c r="C422" s="3"/>
       <c r="D422" s="18"/>
       <c r="E422" s="18"/>
-      <c r="F422" s="216"/>
+      <c r="F422" s="217"/>
       <c r="G422" s="35"/>
       <c r="H422" s="35"/>
       <c r="I422" s="14"/>
@@ -10098,7 +9922,7 @@
       <c r="C423" s="202"/>
       <c r="D423" s="18"/>
       <c r="E423" s="18"/>
-      <c r="F423" s="216"/>
+      <c r="F423" s="217"/>
       <c r="G423" s="35"/>
       <c r="H423" s="35"/>
       <c r="I423" s="14"/>
@@ -10117,7 +9941,7 @@
       <c r="C424" s="202"/>
       <c r="D424" s="14"/>
       <c r="E424" s="18"/>
-      <c r="F424" s="216"/>
+      <c r="F424" s="217"/>
       <c r="G424" s="35"/>
       <c r="H424" s="35"/>
       <c r="I424" s="14"/>
@@ -12226,7 +12050,7 @@
       <c r="C535" s="195"/>
       <c r="D535" s="17"/>
       <c r="E535" s="17"/>
-      <c r="F535" s="218"/>
+      <c r="F535" s="219"/>
       <c r="G535" s="35"/>
       <c r="H535" s="35"/>
       <c r="I535" s="14"/>
@@ -12245,7 +12069,7 @@
       <c r="C536" s="195"/>
       <c r="D536" s="17"/>
       <c r="E536" s="17"/>
-      <c r="F536" s="218"/>
+      <c r="F536" s="219"/>
       <c r="G536" s="35"/>
       <c r="H536" s="35"/>
       <c r="I536" s="14"/>
@@ -12264,7 +12088,7 @@
       <c r="C537" s="195"/>
       <c r="D537" s="17"/>
       <c r="E537" s="17"/>
-      <c r="F537" s="218"/>
+      <c r="F537" s="219"/>
       <c r="G537" s="35"/>
       <c r="H537" s="35"/>
       <c r="I537" s="14"/>
@@ -12283,7 +12107,7 @@
       <c r="C538" s="195"/>
       <c r="D538" s="17"/>
       <c r="E538" s="17"/>
-      <c r="F538" s="218"/>
+      <c r="F538" s="219"/>
       <c r="G538" s="35"/>
       <c r="H538" s="35"/>
       <c r="I538" s="14"/>
@@ -12302,7 +12126,7 @@
       <c r="C539" s="195"/>
       <c r="D539" s="17"/>
       <c r="E539" s="33"/>
-      <c r="F539" s="218"/>
+      <c r="F539" s="219"/>
       <c r="G539" s="35"/>
       <c r="H539" s="35"/>
       <c r="I539" s="14"/>
@@ -12321,7 +12145,7 @@
       <c r="C540" s="195"/>
       <c r="D540" s="17"/>
       <c r="E540" s="33"/>
-      <c r="F540" s="218"/>
+      <c r="F540" s="219"/>
       <c r="G540" s="35"/>
       <c r="H540" s="35"/>
       <c r="I540" s="14"/>
@@ -12340,7 +12164,7 @@
       <c r="C541" s="195"/>
       <c r="D541" s="17"/>
       <c r="E541" s="33"/>
-      <c r="F541" s="218"/>
+      <c r="F541" s="219"/>
       <c r="G541" s="35"/>
       <c r="H541" s="35"/>
       <c r="I541" s="14"/>
@@ -12359,7 +12183,7 @@
       <c r="C542" s="195"/>
       <c r="D542" s="17"/>
       <c r="E542" s="33"/>
-      <c r="F542" s="218"/>
+      <c r="F542" s="219"/>
       <c r="G542" s="35"/>
       <c r="H542" s="35"/>
       <c r="I542" s="14"/>
@@ -12910,7 +12734,7 @@
       <c r="C571" s="195"/>
       <c r="D571" s="17"/>
       <c r="E571" s="17"/>
-      <c r="F571" s="218"/>
+      <c r="F571" s="219"/>
       <c r="G571" s="35"/>
       <c r="H571" s="35"/>
       <c r="I571" s="14"/>
@@ -12929,7 +12753,7 @@
       <c r="C572" s="195"/>
       <c r="D572" s="17"/>
       <c r="E572" s="17"/>
-      <c r="F572" s="218"/>
+      <c r="F572" s="219"/>
       <c r="G572" s="35"/>
       <c r="H572" s="35"/>
       <c r="I572" s="14"/>
@@ -12948,7 +12772,7 @@
       <c r="C573" s="195"/>
       <c r="D573" s="17"/>
       <c r="E573" s="17"/>
-      <c r="F573" s="218"/>
+      <c r="F573" s="219"/>
       <c r="G573" s="35"/>
       <c r="H573" s="35"/>
       <c r="I573" s="14"/>
@@ -12967,7 +12791,7 @@
       <c r="C574" s="195"/>
       <c r="D574" s="17"/>
       <c r="E574" s="17"/>
-      <c r="F574" s="218"/>
+      <c r="F574" s="219"/>
       <c r="G574" s="35"/>
       <c r="H574" s="35"/>
       <c r="I574" s="14"/>
@@ -12986,7 +12810,7 @@
       <c r="C575" s="195"/>
       <c r="D575" s="17"/>
       <c r="E575" s="33"/>
-      <c r="F575" s="218"/>
+      <c r="F575" s="219"/>
       <c r="G575" s="35"/>
       <c r="H575" s="35"/>
       <c r="I575" s="14"/>
@@ -13005,7 +12829,7 @@
       <c r="C576" s="195"/>
       <c r="D576" s="17"/>
       <c r="E576" s="33"/>
-      <c r="F576" s="218"/>
+      <c r="F576" s="219"/>
       <c r="G576" s="35"/>
       <c r="H576" s="35"/>
       <c r="I576" s="14"/>
@@ -13024,7 +12848,7 @@
       <c r="C577" s="195"/>
       <c r="D577" s="17"/>
       <c r="E577" s="33"/>
-      <c r="F577" s="218"/>
+      <c r="F577" s="219"/>
       <c r="G577" s="35"/>
       <c r="H577" s="35"/>
       <c r="I577" s="14"/>
@@ -13043,7 +12867,7 @@
       <c r="C578" s="195"/>
       <c r="D578" s="17"/>
       <c r="E578" s="33"/>
-      <c r="F578" s="218"/>
+      <c r="F578" s="219"/>
       <c r="G578" s="35"/>
       <c r="H578" s="35"/>
       <c r="I578" s="14"/>
@@ -13309,7 +13133,7 @@
       <c r="C592" s="202"/>
       <c r="D592" s="18"/>
       <c r="E592" s="18"/>
-      <c r="F592" s="216"/>
+      <c r="F592" s="217"/>
       <c r="G592" s="35"/>
       <c r="H592" s="71"/>
       <c r="I592" s="47"/>
@@ -15380,7 +15204,7 @@
       <c r="C701" s="11"/>
       <c r="D701" s="27"/>
       <c r="E701" s="11"/>
-      <c r="F701" s="219"/>
+      <c r="F701" s="220"/>
       <c r="G701" s="35"/>
       <c r="H701" s="72"/>
       <c r="I701" s="27"/>
@@ -15399,7 +15223,7 @@
       <c r="C702" s="11"/>
       <c r="D702" s="27"/>
       <c r="E702" s="27"/>
-      <c r="F702" s="219"/>
+      <c r="F702" s="220"/>
       <c r="G702" s="35"/>
       <c r="H702" s="72"/>
       <c r="I702" s="27"/>
@@ -15418,7 +15242,7 @@
       <c r="C703" s="11"/>
       <c r="D703" s="27"/>
       <c r="E703" s="27"/>
-      <c r="F703" s="219"/>
+      <c r="F703" s="220"/>
       <c r="G703" s="35"/>
       <c r="H703" s="72"/>
       <c r="I703" s="27"/>
@@ -15437,7 +15261,7 @@
       <c r="C704" s="11"/>
       <c r="D704" s="27"/>
       <c r="E704" s="27"/>
-      <c r="F704" s="219"/>
+      <c r="F704" s="220"/>
       <c r="G704" s="35"/>
       <c r="H704" s="72"/>
       <c r="I704" s="27"/>
@@ -15456,7 +15280,7 @@
       <c r="C705" s="11"/>
       <c r="D705" s="27"/>
       <c r="E705" s="27"/>
-      <c r="F705" s="219"/>
+      <c r="F705" s="220"/>
       <c r="G705" s="35"/>
       <c r="H705" s="72"/>
       <c r="I705" s="27"/>
@@ -15475,7 +15299,7 @@
       <c r="C706" s="11"/>
       <c r="D706" s="27"/>
       <c r="E706" s="27"/>
-      <c r="F706" s="219"/>
+      <c r="F706" s="220"/>
       <c r="G706" s="35"/>
       <c r="H706" s="72"/>
       <c r="I706" s="27"/>
@@ -15494,7 +15318,7 @@
       <c r="C707" s="11"/>
       <c r="D707" s="27"/>
       <c r="E707" s="27"/>
-      <c r="F707" s="219"/>
+      <c r="F707" s="220"/>
       <c r="G707" s="35"/>
       <c r="H707" s="72"/>
       <c r="I707" s="27"/>
@@ -15513,7 +15337,7 @@
       <c r="C708" s="11"/>
       <c r="D708" s="27"/>
       <c r="E708" s="27"/>
-      <c r="F708" s="219"/>
+      <c r="F708" s="220"/>
       <c r="G708" s="35"/>
       <c r="H708" s="72"/>
       <c r="I708" s="27"/>
@@ -15532,7 +15356,7 @@
       <c r="C709" s="11"/>
       <c r="D709" s="27"/>
       <c r="E709" s="27"/>
-      <c r="F709" s="219"/>
+      <c r="F709" s="220"/>
       <c r="G709" s="35"/>
       <c r="H709" s="72"/>
       <c r="I709" s="27"/>
@@ -15551,7 +15375,7 @@
       <c r="C710" s="11"/>
       <c r="D710" s="27"/>
       <c r="E710" s="27"/>
-      <c r="F710" s="219"/>
+      <c r="F710" s="220"/>
       <c r="G710" s="35"/>
       <c r="H710" s="72"/>
       <c r="I710" s="27"/>
@@ -15570,7 +15394,7 @@
       <c r="C711" s="11"/>
       <c r="D711" s="27"/>
       <c r="E711" s="27"/>
-      <c r="F711" s="219"/>
+      <c r="F711" s="220"/>
       <c r="G711" s="35"/>
       <c r="H711" s="72"/>
       <c r="I711" s="27"/>
@@ -15589,7 +15413,7 @@
       <c r="C712" s="11"/>
       <c r="D712" s="27"/>
       <c r="E712" s="27"/>
-      <c r="F712" s="219"/>
+      <c r="F712" s="220"/>
       <c r="G712" s="35"/>
       <c r="H712" s="72"/>
       <c r="I712" s="27"/>
@@ -15608,7 +15432,7 @@
       <c r="C713" s="11"/>
       <c r="D713" s="27"/>
       <c r="E713" s="27"/>
-      <c r="F713" s="219"/>
+      <c r="F713" s="220"/>
       <c r="G713" s="35"/>
       <c r="H713" s="72"/>
       <c r="I713" s="27"/>
@@ -15627,7 +15451,7 @@
       <c r="C714" s="11"/>
       <c r="D714" s="27"/>
       <c r="E714" s="27"/>
-      <c r="F714" s="219"/>
+      <c r="F714" s="220"/>
       <c r="G714" s="35"/>
       <c r="H714" s="72"/>
       <c r="I714" s="27"/>

</xml_diff>